<commit_message>
[dev] update before report
</commit_message>
<xml_diff>
--- a/src/main/resources/DHKTPM14A_Danhsach.xlsx
+++ b/src/main/resources/DHKTPM14A_Danhsach.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="288" uniqueCount="152">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="270" uniqueCount="143">
   <si>
     <t>Bùi Thành Nam</t>
   </si>
@@ -90,24 +90,15 @@
     <t>Lại Văn Vượng</t>
   </si>
   <si>
-    <t>Lưu Tuấn Kha</t>
-  </si>
-  <si>
     <t>Mã Vũ Tố Trâm</t>
   </si>
   <si>
-    <t>Mai Kiên Cường</t>
-  </si>
-  <si>
     <t>Mai Thanh Trọng</t>
   </si>
   <si>
     <t>Ngô Quang Long</t>
   </si>
   <si>
-    <t>Nguyễn Công Thành Đạt</t>
-  </si>
-  <si>
     <t>Nguyễn Duy Thiện</t>
   </si>
   <si>
@@ -216,9 +207,6 @@
     <t>Trần Vũ Hoàng Sơn</t>
   </si>
   <si>
-    <t>Trương Công Cường</t>
-  </si>
-  <si>
     <t>Trương Đình Phước</t>
   </si>
   <si>
@@ -312,24 +300,15 @@
     <t>0395071374</t>
   </si>
   <si>
-    <t>0983860511</t>
-  </si>
-  <si>
     <t>01636057662</t>
   </si>
   <si>
-    <t>0961516941</t>
-  </si>
-  <si>
     <t>0925562559</t>
   </si>
   <si>
     <t>0846762427</t>
   </si>
   <si>
-    <t>0912366093</t>
-  </si>
-  <si>
     <t>01633021348</t>
   </si>
   <si>
@@ -432,9 +411,6 @@
     <t>0968900475</t>
   </si>
   <si>
-    <t>0961940832</t>
-  </si>
-  <si>
     <t>0702704302</t>
   </si>
   <si>
@@ -472,9 +448,6 @@
   </si>
   <si>
     <t>pass</t>
-  </si>
-  <si>
-    <t>admin</t>
   </si>
 </sst>
 </file>
@@ -869,10 +842,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J73"/>
+  <dimension ref="A1:J66"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A57" workbookViewId="0">
-      <selection activeCell="H73" sqref="H73"/>
+    <sheetView tabSelected="1" topLeftCell="A49" workbookViewId="0">
+      <selection activeCell="H58" sqref="H58"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -898,7 +871,7 @@
         <v>18055471</v>
       </c>
       <c r="D1" s="10" t="s">
-        <v>75</v>
+        <v>71</v>
       </c>
       <c r="E1" s="9">
         <v>72</v>
@@ -907,16 +880,16 @@
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H1" t="s">
-        <v>145</v>
+        <v>137</v>
       </c>
       <c r="I1">
         <v>123456</v>
       </c>
       <c r="J1" t="s">
-        <v>150</v>
+        <v>142</v>
       </c>
     </row>
     <row r="2" spans="1:10" x14ac:dyDescent="0.25">
@@ -930,7 +903,7 @@
         <v>18084851</v>
       </c>
       <c r="D2" s="10" t="s">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="E2" s="9">
         <v>72</v>
@@ -939,7 +912,7 @@
         <v>1</v>
       </c>
       <c r="G2" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I2">
         <v>123456</v>
@@ -956,7 +929,7 @@
         <v>18087531</v>
       </c>
       <c r="D3" s="10" t="s">
-        <v>77</v>
+        <v>73</v>
       </c>
       <c r="E3" s="9">
         <v>72</v>
@@ -965,7 +938,7 @@
         <v>1</v>
       </c>
       <c r="G3" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I3">
         <v>123456</v>
@@ -982,7 +955,7 @@
         <v>18062161</v>
       </c>
       <c r="D4" s="10" t="s">
-        <v>78</v>
+        <v>74</v>
       </c>
       <c r="E4" s="9">
         <v>72</v>
@@ -991,10 +964,10 @@
         <v>1</v>
       </c>
       <c r="G4" s="1" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="H4" t="s">
-        <v>146</v>
+        <v>138</v>
       </c>
       <c r="I4">
         <v>123456</v>
@@ -1011,7 +984,7 @@
         <v>18025441</v>
       </c>
       <c r="D5" s="10" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="E5" s="9">
         <v>72</v>
@@ -1020,7 +993,7 @@
         <v>1</v>
       </c>
       <c r="G5" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I5">
         <v>123456</v>
@@ -1037,7 +1010,7 @@
         <v>18086981</v>
       </c>
       <c r="D6" s="10" t="s">
-        <v>80</v>
+        <v>76</v>
       </c>
       <c r="E6" s="9">
         <v>70</v>
@@ -1046,7 +1019,7 @@
         <v>1</v>
       </c>
       <c r="G6" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I6">
         <v>123456</v>
@@ -1063,7 +1036,7 @@
         <v>18065321</v>
       </c>
       <c r="D7" s="10" t="s">
-        <v>81</v>
+        <v>77</v>
       </c>
       <c r="E7" s="9">
         <v>68</v>
@@ -1072,10 +1045,10 @@
         <v>1</v>
       </c>
       <c r="G7" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H7" t="s">
-        <v>147</v>
+        <v>139</v>
       </c>
       <c r="I7">
         <v>123456</v>
@@ -1092,7 +1065,7 @@
         <v>18040671</v>
       </c>
       <c r="D8" s="10" t="s">
-        <v>82</v>
+        <v>78</v>
       </c>
       <c r="E8" s="9">
         <v>76</v>
@@ -1101,7 +1074,7 @@
         <v>1</v>
       </c>
       <c r="G8" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I8">
         <v>123456</v>
@@ -1118,7 +1091,7 @@
         <v>18024491</v>
       </c>
       <c r="D9" s="10" t="s">
-        <v>83</v>
+        <v>79</v>
       </c>
       <c r="E9" s="9">
         <v>72</v>
@@ -1127,7 +1100,7 @@
         <v>1</v>
       </c>
       <c r="G9" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I9">
         <v>123456</v>
@@ -1144,7 +1117,7 @@
         <v>18056521</v>
       </c>
       <c r="D10" s="10" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="E10" s="9">
         <v>76</v>
@@ -1153,10 +1126,10 @@
         <v>1</v>
       </c>
       <c r="G10" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H10" t="s">
-        <v>148</v>
+        <v>140</v>
       </c>
       <c r="I10">
         <v>123456</v>
@@ -1173,7 +1146,7 @@
         <v>18050901</v>
       </c>
       <c r="D11" s="10" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
       <c r="E11" s="9">
         <v>72</v>
@@ -1182,7 +1155,7 @@
         <v>1</v>
       </c>
       <c r="G11" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I11">
         <v>123456</v>
@@ -1199,7 +1172,7 @@
         <v>18025261</v>
       </c>
       <c r="D12" s="10" t="s">
-        <v>86</v>
+        <v>82</v>
       </c>
       <c r="E12" s="9">
         <v>74</v>
@@ -1208,7 +1181,7 @@
         <v>1</v>
       </c>
       <c r="G12" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I12">
         <v>123456</v>
@@ -1225,7 +1198,7 @@
         <v>18065341</v>
       </c>
       <c r="D13" s="10" t="s">
-        <v>87</v>
+        <v>83</v>
       </c>
       <c r="E13" s="9">
         <v>74</v>
@@ -1234,7 +1207,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I13">
         <v>123456</v>
@@ -1251,7 +1224,7 @@
         <v>18019301</v>
       </c>
       <c r="D14" s="10" t="s">
-        <v>88</v>
+        <v>84</v>
       </c>
       <c r="E14" s="9">
         <v>72</v>
@@ -1260,10 +1233,10 @@
         <v>1</v>
       </c>
       <c r="G14" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H14" t="s">
-        <v>149</v>
+        <v>141</v>
       </c>
       <c r="I14">
         <v>123456</v>
@@ -1280,7 +1253,7 @@
         <v>18037851</v>
       </c>
       <c r="D15" s="10" t="s">
-        <v>89</v>
+        <v>85</v>
       </c>
       <c r="E15" s="9">
         <v>72</v>
@@ -1289,7 +1262,7 @@
         <v>1</v>
       </c>
       <c r="G15" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I15">
         <v>123456</v>
@@ -1306,7 +1279,7 @@
         <v>18053681</v>
       </c>
       <c r="D16" s="10" t="s">
-        <v>90</v>
+        <v>86</v>
       </c>
       <c r="E16" s="9">
         <v>74</v>
@@ -1315,7 +1288,7 @@
         <v>1</v>
       </c>
       <c r="G16" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I16">
         <v>123456</v>
@@ -1332,7 +1305,7 @@
         <v>18048941</v>
       </c>
       <c r="D17" s="10" t="s">
-        <v>91</v>
+        <v>87</v>
       </c>
       <c r="E17" s="9">
         <v>76</v>
@@ -1341,7 +1314,7 @@
         <v>1</v>
       </c>
       <c r="G17" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I17">
         <v>123456</v>
@@ -1358,7 +1331,7 @@
         <v>18040321</v>
       </c>
       <c r="D18" s="10" t="s">
-        <v>92</v>
+        <v>88</v>
       </c>
       <c r="E18" s="9">
         <v>78</v>
@@ -1367,7 +1340,7 @@
         <v>1</v>
       </c>
       <c r="G18" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I18">
         <v>123456</v>
@@ -1384,7 +1357,7 @@
         <v>18028161</v>
       </c>
       <c r="D19" s="10" t="s">
-        <v>93</v>
+        <v>89</v>
       </c>
       <c r="E19" s="9">
         <v>72</v>
@@ -1393,7 +1366,7 @@
         <v>1</v>
       </c>
       <c r="G19" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I19">
         <v>123456</v>
@@ -1410,7 +1383,7 @@
         <v>18045551</v>
       </c>
       <c r="D20" s="10" t="s">
-        <v>94</v>
+        <v>90</v>
       </c>
       <c r="E20" s="9">
         <v>74</v>
@@ -1419,7 +1392,7 @@
         <v>1</v>
       </c>
       <c r="G20" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I20">
         <v>123456</v>
@@ -1436,7 +1409,7 @@
         <v>18093421</v>
       </c>
       <c r="D21" s="10" t="s">
-        <v>95</v>
+        <v>91</v>
       </c>
       <c r="E21" s="9">
         <v>72</v>
@@ -1445,7 +1418,7 @@
         <v>1</v>
       </c>
       <c r="G21" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I21">
         <v>123456</v>
@@ -1462,7 +1435,7 @@
         <v>18072661</v>
       </c>
       <c r="D22" s="10" t="s">
-        <v>96</v>
+        <v>92</v>
       </c>
       <c r="E22" s="9">
         <v>72</v>
@@ -1471,7 +1444,7 @@
         <v>1</v>
       </c>
       <c r="G22" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I22">
         <v>123456</v>
@@ -1485,19 +1458,19 @@
         <v>23</v>
       </c>
       <c r="C23" s="8">
-        <v>18093751</v>
+        <v>18055381</v>
       </c>
       <c r="D23" s="10" t="s">
-        <v>97</v>
+        <v>93</v>
       </c>
       <c r="E23" s="9">
-        <v>68</v>
+        <v>65</v>
       </c>
       <c r="F23" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G23" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I23">
         <v>123456</v>
@@ -1511,19 +1484,19 @@
         <v>24</v>
       </c>
       <c r="C24" s="8">
-        <v>18055381</v>
+        <v>18064861</v>
       </c>
       <c r="D24" s="10" t="s">
-        <v>98</v>
+        <v>94</v>
       </c>
       <c r="E24" s="9">
-        <v>65</v>
+        <v>74</v>
       </c>
       <c r="F24" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G24" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I24">
         <v>123456</v>
@@ -1537,19 +1510,19 @@
         <v>25</v>
       </c>
       <c r="C25" s="8">
-        <v>18089811</v>
+        <v>18039011</v>
       </c>
       <c r="D25" s="10" t="s">
-        <v>99</v>
+        <v>95</v>
       </c>
       <c r="E25" s="9">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F25" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G25" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I25">
         <v>123456</v>
@@ -1563,19 +1536,19 @@
         <v>26</v>
       </c>
       <c r="C26" s="8">
-        <v>18064861</v>
+        <v>18087521</v>
       </c>
       <c r="D26" s="10" t="s">
-        <v>100</v>
+        <v>96</v>
       </c>
       <c r="E26" s="9">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F26" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G26" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I26">
         <v>123456</v>
@@ -1589,25 +1562,25 @@
         <v>27</v>
       </c>
       <c r="C27" s="8">
-        <v>18039011</v>
+        <v>18090621</v>
       </c>
       <c r="D27" s="10" t="s">
-        <v>101</v>
+        <v>97</v>
       </c>
       <c r="E27" s="9">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F27" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G27" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I27">
         <v>123456</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A28" s="6">
         <v>28</v>
       </c>
@@ -1615,10 +1588,10 @@
         <v>28</v>
       </c>
       <c r="C28" s="8">
-        <v>18081331</v>
+        <v>18058151</v>
       </c>
       <c r="D28" s="10" t="s">
-        <v>102</v>
+        <v>98</v>
       </c>
       <c r="E28" s="9">
         <v>72</v>
@@ -1627,7 +1600,7 @@
         <v>1</v>
       </c>
       <c r="G28" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I28">
         <v>123456</v>
@@ -1641,25 +1614,25 @@
         <v>29</v>
       </c>
       <c r="C29" s="8">
-        <v>18087521</v>
+        <v>18040711</v>
       </c>
       <c r="D29" s="10" t="s">
-        <v>103</v>
+        <v>99</v>
       </c>
       <c r="E29" s="9">
-        <v>70</v>
+        <v>75</v>
       </c>
       <c r="F29" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G29" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I29">
         <v>123456</v>
       </c>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A30" s="6">
         <v>30</v>
       </c>
@@ -1667,19 +1640,19 @@
         <v>30</v>
       </c>
       <c r="C30" s="8">
-        <v>18090621</v>
+        <v>18077551</v>
       </c>
       <c r="D30" s="10" t="s">
-        <v>104</v>
+        <v>100</v>
       </c>
       <c r="E30" s="9">
-        <v>68</v>
+        <v>72</v>
       </c>
       <c r="F30" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G30" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I30">
         <v>123456</v>
@@ -1693,10 +1666,10 @@
         <v>31</v>
       </c>
       <c r="C31" s="8">
-        <v>18058151</v>
+        <v>18087991</v>
       </c>
       <c r="D31" s="10" t="s">
-        <v>105</v>
+        <v>101</v>
       </c>
       <c r="E31" s="9">
         <v>72</v>
@@ -1705,7 +1678,7 @@
         <v>1</v>
       </c>
       <c r="G31" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I31">
         <v>123456</v>
@@ -1719,10 +1692,10 @@
         <v>32</v>
       </c>
       <c r="C32" s="8">
-        <v>18040711</v>
+        <v>18069461</v>
       </c>
       <c r="D32" s="10" t="s">
-        <v>106</v>
+        <v>102</v>
       </c>
       <c r="E32" s="9">
         <v>75</v>
@@ -1731,13 +1704,13 @@
         <v>1</v>
       </c>
       <c r="G32" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I32">
         <v>123456</v>
       </c>
     </row>
-    <row r="33" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="6">
         <v>33</v>
       </c>
@@ -1745,19 +1718,19 @@
         <v>33</v>
       </c>
       <c r="C33" s="8">
-        <v>18077551</v>
+        <v>18085541</v>
       </c>
       <c r="D33" s="10" t="s">
-        <v>107</v>
+        <v>103</v>
       </c>
       <c r="E33" s="9">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F33" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G33" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I33">
         <v>123456</v>
@@ -1771,19 +1744,19 @@
         <v>34</v>
       </c>
       <c r="C34" s="8">
-        <v>18087991</v>
+        <v>18080931</v>
       </c>
       <c r="D34" s="10" t="s">
-        <v>108</v>
+        <v>104</v>
       </c>
       <c r="E34" s="9">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F34" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G34" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I34">
         <v>123456</v>
@@ -1797,25 +1770,25 @@
         <v>35</v>
       </c>
       <c r="C35" s="8">
-        <v>18069461</v>
+        <v>18094051</v>
       </c>
       <c r="D35" s="10" t="s">
-        <v>109</v>
+        <v>105</v>
       </c>
       <c r="E35" s="9">
-        <v>75</v>
+        <v>70</v>
       </c>
       <c r="F35" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G35" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I35">
         <v>123456</v>
       </c>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A36" s="6">
         <v>36</v>
       </c>
@@ -1823,19 +1796,19 @@
         <v>36</v>
       </c>
       <c r="C36" s="8">
-        <v>18085541</v>
+        <v>18090321</v>
       </c>
       <c r="D36" s="10" t="s">
-        <v>110</v>
+        <v>106</v>
       </c>
       <c r="E36" s="9">
-        <v>68</v>
+        <v>63</v>
       </c>
       <c r="F36" s="9" t="s">
-        <v>1</v>
+        <v>37</v>
       </c>
       <c r="G36" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I36">
         <v>123456</v>
@@ -1846,22 +1819,22 @@
         <v>37</v>
       </c>
       <c r="B37" s="7" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C37" s="8">
-        <v>18080931</v>
+        <v>18052451</v>
       </c>
       <c r="D37" s="10" t="s">
-        <v>111</v>
+        <v>107</v>
       </c>
       <c r="E37" s="9">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F37" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G37" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I37">
         <v>123456</v>
@@ -1872,48 +1845,48 @@
         <v>38</v>
       </c>
       <c r="B38" s="7" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="C38" s="8">
-        <v>18094051</v>
+        <v>18029181</v>
       </c>
       <c r="D38" s="10" t="s">
-        <v>112</v>
+        <v>108</v>
       </c>
       <c r="E38" s="9">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F38" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G38" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I38">
         <v>123456</v>
       </c>
     </row>
-    <row r="39" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="6">
         <v>39</v>
       </c>
       <c r="B39" s="7" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C39" s="8">
-        <v>18090321</v>
+        <v>18058581</v>
       </c>
       <c r="D39" s="10" t="s">
-        <v>113</v>
+        <v>109</v>
       </c>
       <c r="E39" s="9">
-        <v>63</v>
+        <v>75</v>
       </c>
       <c r="F39" s="9" t="s">
-        <v>40</v>
+        <v>1</v>
       </c>
       <c r="G39" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I39">
         <v>123456</v>
@@ -1927,25 +1900,25 @@
         <v>41</v>
       </c>
       <c r="C40" s="8">
-        <v>18052451</v>
+        <v>18036401</v>
       </c>
       <c r="D40" s="10" t="s">
-        <v>114</v>
+        <v>110</v>
       </c>
       <c r="E40" s="9">
-        <v>76</v>
+        <v>72</v>
       </c>
       <c r="F40" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G40" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I40">
         <v>123456</v>
       </c>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A41" s="6">
         <v>41</v>
       </c>
@@ -1953,10 +1926,10 @@
         <v>42</v>
       </c>
       <c r="C41" s="8">
-        <v>18029181</v>
+        <v>18068061</v>
       </c>
       <c r="D41" s="10" t="s">
-        <v>115</v>
+        <v>111</v>
       </c>
       <c r="E41" s="9">
         <v>72</v>
@@ -1965,7 +1938,7 @@
         <v>1</v>
       </c>
       <c r="G41" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I41">
         <v>123456</v>
@@ -1979,25 +1952,25 @@
         <v>43</v>
       </c>
       <c r="C42" s="8">
-        <v>18058581</v>
+        <v>18076131</v>
       </c>
       <c r="D42" s="10" t="s">
-        <v>116</v>
+        <v>112</v>
       </c>
       <c r="E42" s="9">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="F42" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G42" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I42">
         <v>123456</v>
       </c>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A43" s="6">
         <v>43</v>
       </c>
@@ -2005,19 +1978,19 @@
         <v>44</v>
       </c>
       <c r="C43" s="8">
-        <v>18036401</v>
+        <v>18062811</v>
       </c>
       <c r="D43" s="10" t="s">
-        <v>117</v>
+        <v>113</v>
       </c>
       <c r="E43" s="9">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F43" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G43" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I43">
         <v>123456</v>
@@ -2031,19 +2004,19 @@
         <v>45</v>
       </c>
       <c r="C44" s="8">
-        <v>18068061</v>
+        <v>18036971</v>
       </c>
       <c r="D44" s="10" t="s">
-        <v>118</v>
+        <v>114</v>
       </c>
       <c r="E44" s="9">
-        <v>72</v>
+        <v>84</v>
       </c>
       <c r="F44" s="9" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="G44" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I44">
         <v>123456</v>
@@ -2054,74 +2027,74 @@
         <v>45</v>
       </c>
       <c r="B45" s="7" t="s">
+        <v>47</v>
+      </c>
+      <c r="C45" s="8">
+        <v>18065371</v>
+      </c>
+      <c r="D45" s="10" t="s">
+        <v>115</v>
+      </c>
+      <c r="E45" s="9">
+        <v>80</v>
+      </c>
+      <c r="F45" s="9" t="s">
         <v>46</v>
       </c>
-      <c r="C45" s="8">
-        <v>18076131</v>
-      </c>
-      <c r="D45" s="10" t="s">
-        <v>119</v>
-      </c>
-      <c r="E45" s="9">
-        <v>77</v>
-      </c>
-      <c r="F45" s="9" t="s">
-        <v>1</v>
-      </c>
       <c r="G45" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I45">
         <v>123456</v>
       </c>
     </row>
-    <row r="46" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A46" s="6">
         <v>46</v>
       </c>
       <c r="B46" s="7" t="s">
-        <v>47</v>
+        <v>48</v>
       </c>
       <c r="C46" s="8">
-        <v>18062811</v>
+        <v>18042041</v>
       </c>
       <c r="D46" s="10" t="s">
-        <v>120</v>
+        <v>116</v>
       </c>
       <c r="E46" s="9">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="F46" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G46" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I46">
         <v>123456</v>
       </c>
     </row>
-    <row r="47" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="6">
         <v>47</v>
       </c>
       <c r="B47" s="7" t="s">
-        <v>48</v>
+        <v>49</v>
       </c>
       <c r="C47" s="8">
-        <v>18036971</v>
+        <v>18086141</v>
       </c>
       <c r="D47" s="10" t="s">
-        <v>121</v>
+        <v>117</v>
       </c>
       <c r="E47" s="9">
-        <v>84</v>
+        <v>68</v>
       </c>
       <c r="F47" s="9" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G47" s="1" t="s">
-        <v>73</v>
+        <v>70</v>
       </c>
       <c r="I47">
         <v>123456</v>
@@ -2135,19 +2108,19 @@
         <v>50</v>
       </c>
       <c r="C48" s="8">
-        <v>18065371</v>
+        <v>18043151</v>
       </c>
       <c r="D48" s="10" t="s">
-        <v>122</v>
+        <v>118</v>
       </c>
       <c r="E48" s="9">
-        <v>80</v>
+        <v>72</v>
       </c>
       <c r="F48" s="9" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G48" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I48">
         <v>123456</v>
@@ -2161,19 +2134,19 @@
         <v>51</v>
       </c>
       <c r="C49" s="8">
-        <v>18042041</v>
+        <v>18061351</v>
       </c>
       <c r="D49" s="10" t="s">
-        <v>123</v>
+        <v>119</v>
       </c>
       <c r="E49" s="9">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="F49" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G49" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I49">
         <v>123456</v>
@@ -2187,19 +2160,19 @@
         <v>52</v>
       </c>
       <c r="C50" s="8">
-        <v>18086141</v>
+        <v>18076801</v>
       </c>
       <c r="D50" s="10" t="s">
-        <v>124</v>
+        <v>120</v>
       </c>
       <c r="E50" s="9">
-        <v>68</v>
+        <v>75</v>
       </c>
       <c r="F50" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G50" s="1" t="s">
-        <v>74</v>
+        <v>69</v>
       </c>
       <c r="I50">
         <v>123456</v>
@@ -2213,19 +2186,19 @@
         <v>53</v>
       </c>
       <c r="C51" s="8">
-        <v>18043151</v>
+        <v>18038171</v>
       </c>
       <c r="D51" s="10" t="s">
-        <v>125</v>
+        <v>121</v>
       </c>
       <c r="E51" s="9">
-        <v>72</v>
+        <v>82</v>
       </c>
       <c r="F51" s="9" t="s">
-        <v>1</v>
+        <v>46</v>
       </c>
       <c r="G51" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I51">
         <v>123456</v>
@@ -2239,10 +2212,10 @@
         <v>54</v>
       </c>
       <c r="C52" s="8">
-        <v>18061351</v>
+        <v>18037481</v>
       </c>
       <c r="D52" s="10" t="s">
-        <v>126</v>
+        <v>122</v>
       </c>
       <c r="E52" s="9">
         <v>72</v>
@@ -2251,7 +2224,7 @@
         <v>1</v>
       </c>
       <c r="G52" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I52">
         <v>123456</v>
@@ -2265,19 +2238,19 @@
         <v>55</v>
       </c>
       <c r="C53" s="8">
-        <v>18076801</v>
+        <v>18031221</v>
       </c>
       <c r="D53" s="10" t="s">
-        <v>127</v>
+        <v>123</v>
       </c>
       <c r="E53" s="9">
-        <v>75</v>
+        <v>72</v>
       </c>
       <c r="F53" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G53" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I53">
         <v>123456</v>
@@ -2291,19 +2264,19 @@
         <v>56</v>
       </c>
       <c r="C54" s="8">
-        <v>18038171</v>
+        <v>18037141</v>
       </c>
       <c r="D54" s="10" t="s">
-        <v>128</v>
+        <v>124</v>
       </c>
       <c r="E54" s="9">
-        <v>82</v>
+        <v>72</v>
       </c>
       <c r="F54" s="9" t="s">
-        <v>49</v>
+        <v>1</v>
       </c>
       <c r="G54" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I54">
         <v>123456</v>
@@ -2317,19 +2290,19 @@
         <v>57</v>
       </c>
       <c r="C55" s="8">
-        <v>18037481</v>
+        <v>18049511</v>
       </c>
       <c r="D55" s="10" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
       <c r="E55" s="9">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F55" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G55" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I55">
         <v>123456</v>
@@ -2343,10 +2316,10 @@
         <v>58</v>
       </c>
       <c r="C56" s="8">
-        <v>18031221</v>
+        <v>18083111</v>
       </c>
       <c r="D56" s="10" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="E56" s="9">
         <v>72</v>
@@ -2355,7 +2328,7 @@
         <v>1</v>
       </c>
       <c r="G56" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I56">
         <v>123456</v>
@@ -2369,19 +2342,19 @@
         <v>59</v>
       </c>
       <c r="C57" s="8">
-        <v>18037141</v>
+        <v>18037431</v>
       </c>
       <c r="D57" s="10" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
       <c r="E57" s="9">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F57" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G57" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I57">
         <v>123456</v>
@@ -2395,19 +2368,19 @@
         <v>60</v>
       </c>
       <c r="C58" s="8">
-        <v>18049511</v>
+        <v>18079461</v>
       </c>
       <c r="D58" s="10" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="E58" s="9">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="F58" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G58" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I58">
         <v>123456</v>
@@ -2421,10 +2394,10 @@
         <v>61</v>
       </c>
       <c r="C59" s="8">
-        <v>18083111</v>
+        <v>18028791</v>
       </c>
       <c r="D59" s="10" t="s">
-        <v>133</v>
+        <v>129</v>
       </c>
       <c r="E59" s="9">
         <v>72</v>
@@ -2433,7 +2406,7 @@
         <v>1</v>
       </c>
       <c r="G59" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I59">
         <v>123456</v>
@@ -2447,19 +2420,19 @@
         <v>62</v>
       </c>
       <c r="C60" s="8">
-        <v>18037431</v>
+        <v>18055971</v>
       </c>
       <c r="D60" s="10" t="s">
-        <v>134</v>
+        <v>130</v>
       </c>
       <c r="E60" s="9">
-        <v>68</v>
+        <v>76</v>
       </c>
       <c r="F60" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G60" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I60">
         <v>123456</v>
@@ -2473,10 +2446,10 @@
         <v>63</v>
       </c>
       <c r="C61" s="8">
-        <v>18079461</v>
+        <v>18058511</v>
       </c>
       <c r="D61" s="10" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
       <c r="E61" s="9">
         <v>72</v>
@@ -2485,7 +2458,7 @@
         <v>1</v>
       </c>
       <c r="G61" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I61">
         <v>123456</v>
@@ -2499,10 +2472,10 @@
         <v>64</v>
       </c>
       <c r="C62" s="8">
-        <v>18028791</v>
+        <v>18060441</v>
       </c>
       <c r="D62" s="10" t="s">
-        <v>136</v>
+        <v>132</v>
       </c>
       <c r="E62" s="9">
         <v>72</v>
@@ -2511,7 +2484,7 @@
         <v>1</v>
       </c>
       <c r="G62" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I62">
         <v>123456</v>
@@ -2525,10 +2498,10 @@
         <v>65</v>
       </c>
       <c r="C63" s="8">
-        <v>18084791</v>
+        <v>18058521</v>
       </c>
       <c r="D63" s="10" t="s">
-        <v>137</v>
+        <v>133</v>
       </c>
       <c r="E63" s="9">
         <v>72</v>
@@ -2537,7 +2510,7 @@
         <v>1</v>
       </c>
       <c r="G63" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I63">
         <v>123456</v>
@@ -2551,19 +2524,19 @@
         <v>66</v>
       </c>
       <c r="C64" s="8">
-        <v>18055971</v>
+        <v>18043531</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>138</v>
+        <v>134</v>
       </c>
       <c r="E64" s="9">
-        <v>76</v>
+        <v>68</v>
       </c>
       <c r="F64" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G64" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I64">
         <v>123456</v>
@@ -2577,19 +2550,19 @@
         <v>67</v>
       </c>
       <c r="C65" s="8">
-        <v>18058511</v>
+        <v>18027091</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>139</v>
+        <v>135</v>
       </c>
       <c r="E65" s="9">
-        <v>72</v>
+        <v>68</v>
       </c>
       <c r="F65" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G65" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I65">
         <v>123456</v>
@@ -2603,134 +2576,22 @@
         <v>68</v>
       </c>
       <c r="C66" s="8">
-        <v>18060441</v>
+        <v>18068771</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>140</v>
+        <v>136</v>
       </c>
       <c r="E66" s="9">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="F66" s="9" t="s">
         <v>1</v>
       </c>
       <c r="G66" s="1" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="I66">
         <v>123456</v>
-      </c>
-    </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A67" s="6">
-        <v>67</v>
-      </c>
-      <c r="B67" s="7" t="s">
-        <v>69</v>
-      </c>
-      <c r="C67" s="8">
-        <v>18058521</v>
-      </c>
-      <c r="D67" s="10" t="s">
-        <v>141</v>
-      </c>
-      <c r="E67" s="9">
-        <v>72</v>
-      </c>
-      <c r="F67" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G67" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I67">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A68" s="6">
-        <v>68</v>
-      </c>
-      <c r="B68" s="7" t="s">
-        <v>70</v>
-      </c>
-      <c r="C68" s="8">
-        <v>18043531</v>
-      </c>
-      <c r="D68" s="10" t="s">
-        <v>142</v>
-      </c>
-      <c r="E68" s="9">
-        <v>68</v>
-      </c>
-      <c r="F68" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G68" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I68">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A69" s="6">
-        <v>69</v>
-      </c>
-      <c r="B69" s="7" t="s">
-        <v>71</v>
-      </c>
-      <c r="C69" s="8">
-        <v>18027091</v>
-      </c>
-      <c r="D69" s="10" t="s">
-        <v>143</v>
-      </c>
-      <c r="E69" s="9">
-        <v>68</v>
-      </c>
-      <c r="F69" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G69" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I69">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A70" s="6">
-        <v>70</v>
-      </c>
-      <c r="B70" s="7" t="s">
-        <v>72</v>
-      </c>
-      <c r="C70" s="8">
-        <v>18068771</v>
-      </c>
-      <c r="D70" s="10" t="s">
-        <v>144</v>
-      </c>
-      <c r="E70" s="9">
-        <v>74</v>
-      </c>
-      <c r="F70" s="9" t="s">
-        <v>1</v>
-      </c>
-      <c r="G70" s="1" t="s">
-        <v>73</v>
-      </c>
-      <c r="I70">
-        <v>123456</v>
-      </c>
-    </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="B73" s="4" t="s">
-        <v>151</v>
-      </c>
-      <c r="I73" t="s">
-        <v>151</v>
       </c>
     </row>
   </sheetData>

</xml_diff>